<commit_message>
Introduce core function <kfCore_ts_agg> for generalized time series aggregation
</commit_message>
<xml_diff>
--- a/Python/omniPy/AdvDB/CFG_KPI_Example.xlsx
+++ b/Python/omniPy/AdvDB/CFG_KPI_Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\omniPy\AdvDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFA396A-156C-4550-B92B-043CBB21BA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB81552-4772-45C3-B8BD-A6D3E60AFC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09020CF4-9F51-448A-8C84-8E8C9A006B79}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
   <si>
     <t>D_BGN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -142,6 +142,30 @@
   </si>
   <si>
     <t>{'encoding' : 'GB18030'}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kpi1 roll 15 day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kpi2 roll 15 day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r15_&amp;L_curdate..hdf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kpi2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>130102</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>140112</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -512,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01402B73-73A9-49DD-BA23-F0DAE3D77BCF}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -570,7 +594,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>42370</v>
+        <v>42429</v>
       </c>
       <c r="B2" s="1">
         <v>73050</v>
@@ -602,7 +626,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>42370</v>
+        <v>42429</v>
       </c>
       <c r="B3" s="1">
         <v>73050</v>
@@ -634,7 +658,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>42516</v>
+        <v>42429</v>
       </c>
       <c r="B4" s="1">
         <v>73050</v>
@@ -666,7 +690,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>42516</v>
+        <v>42429</v>
       </c>
       <c r="B5" s="1">
         <v>73050</v>
@@ -698,7 +722,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>42370</v>
+        <v>42429</v>
       </c>
       <c r="B6" s="1">
         <v>73050</v>
@@ -730,7 +754,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>42370</v>
+        <v>42429</v>
       </c>
       <c r="B7" s="1">
         <v>73050</v>
@@ -784,6 +808,70 @@
       </c>
       <c r="I8" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>42429</v>
+      </c>
+      <c r="B9" s="1">
+        <v>73050</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>42516</v>
+      </c>
+      <c r="B10" s="1">
+        <v>73050</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>